<commit_message>
Version 2.3.2: Stable version finale, avec UI et une bdd bien conceptualisés. Limitations: commentaires(ajout et suppression), agilité, l'autre option à explorer
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Users\DELL\Projects\Python\Streamlit\myproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC4B71E3-9CD7-40FA-A19E-762ECB5EF27D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A985075-FCC0-43DE-9E7D-D59CA5776D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="300" windowWidth="14400" windowHeight="7245" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="convection" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="34">
   <si>
     <t>Datetime1</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>Datetime</t>
+  </si>
+  <si>
+    <t>Layer</t>
   </si>
   <si>
     <t>Phenomena_presence</t>
@@ -472,15 +475,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -512,18 +515,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.140625" bestFit="1" customWidth="1"/>
@@ -605,13 +607,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:F1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -644,7 +648,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A2:XFD10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -705,45 +709,45 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AC1"/>
+  <dimension ref="A1:AD1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A2:XFD10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="23.140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -830,6 +834,9 @@
       </c>
       <c r="AC1" t="s">
         <v>32</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stable version finale. Limitations: Ajout des commentaires, Agilité
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Users\DELL\Projects\Python\Streamlit\myproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A985075-FCC0-43DE-9E7D-D59CA5776D64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{159759A7-D65B-4E54-AD4F-67F0524FFB66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19440" windowHeight="10320" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="convection" sheetId="1" r:id="rId1"/>
@@ -475,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,7 +516,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A4" sqref="A2:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -648,7 +648,7 @@
   <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A3" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -711,13 +711,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AD1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" zoomScale="81" workbookViewId="0">
+      <selection activeCell="A11" sqref="A2:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.140625" bestFit="1" customWidth="1"/>

</xml_diff>